<commit_message>
storage model issues sorted
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Time Period</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>PSH</t>
+  </si>
+  <si>
+    <t>PSH2</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
         <v>1900</v>
       </c>
       <c r="C2">
-        <v>4100</v>
+        <v>1100</v>
       </c>
       <c r="D2">
         <v>3000</v>
@@ -480,10 +483,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2100</v>
+        <v>2100.000000000001</v>
       </c>
       <c r="C3">
-        <v>933.3333333333334</v>
+        <v>1600</v>
       </c>
       <c r="D3">
         <v>2700</v>
@@ -494,10 +497,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2300</v>
+        <v>2300.000000000001</v>
       </c>
       <c r="C4">
-        <v>450</v>
+        <v>2598.148148148149</v>
       </c>
       <c r="D4">
         <v>3000</v>
@@ -511,7 +514,7 @@
         <v>2100</v>
       </c>
       <c r="C5">
-        <v>750</v>
+        <v>4148.148148148149</v>
       </c>
       <c r="D5">
         <v>3350</v>
@@ -525,7 +528,7 @@
         <v>2300</v>
       </c>
       <c r="C6">
-        <v>550</v>
+        <v>300.0000000000003</v>
       </c>
       <c r="D6">
         <v>3600</v>
@@ -539,7 +542,7 @@
         <v>2200</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>500.0000000000002</v>
       </c>
       <c r="D7">
         <v>3200</v>
@@ -553,7 +556,7 @@
         <v>2450</v>
       </c>
       <c r="C8">
-        <v>1314.506172839506</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>3550</v>
@@ -567,7 +570,7 @@
         <v>2770</v>
       </c>
       <c r="C9">
-        <v>1514.506172839506</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>3820</v>
@@ -581,7 +584,7 @@
         <v>2750</v>
       </c>
       <c r="C10">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>3700</v>
@@ -592,10 +595,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2800</v>
+        <v>2800.000000000001</v>
       </c>
       <c r="C11">
-        <v>350</v>
+        <v>850.0000000000002</v>
       </c>
       <c r="D11">
         <v>3650</v>
@@ -642,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>4100</v>
+        <v>1100</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -676,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>933.3333333333334</v>
+        <v>1600</v>
       </c>
       <c r="E4">
         <v>500</v>
@@ -690,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2100</v>
+        <v>2100.000000000001</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -710,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>450</v>
+        <v>2598.148148148149</v>
       </c>
       <c r="E6">
         <v>600</v>
@@ -724,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>2300</v>
+        <v>2300.000000000001</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -744,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>750</v>
+        <v>4148.148148148149</v>
       </c>
       <c r="E8">
         <v>1150</v>
@@ -778,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>550</v>
+        <v>300.0000000000003</v>
       </c>
       <c r="E10">
         <v>1200</v>
@@ -812,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>500.0000000000002</v>
       </c>
       <c r="E12">
         <v>900</v>
@@ -846,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1314.506172839506</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -880,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1514.506172839506</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>950</v>
@@ -914,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>850</v>
@@ -948,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>350</v>
+        <v>850.0000000000002</v>
       </c>
       <c r="E20">
         <v>750</v>
@@ -962,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>2800</v>
+        <v>2800.000000000001</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1301,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2100</v>
+        <v>2100.000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1361,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>2300</v>
+        <v>2300.000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1781,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>2800</v>
+        <v>2800.000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1811,7 +1814,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1842,30 +1845,30 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>333.3333333333334</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1873,33 +1876,33 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>-277.7777777777778</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D5">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>-555.5555555555555</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1907,33 +1910,33 @@
         <v>21</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1000.000000000001</v>
       </c>
       <c r="D6">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>-833.3333333333334</v>
+        <v>900.0000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>898.1481481481477</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>-1111.111111111111</v>
+        <v>808.3333333333328</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1941,33 +1944,33 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>214.5061728395063</v>
+        <v>1500.000000000001</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>193.0555555555556</v>
+        <v>1350.000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>464.5061728395062</v>
+        <v>1398.148148148148</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>418.0555555555556</v>
+        <v>1258.333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1975,24 +1978,24 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="E10">
-        <v>-277.7777777777778</v>
+        <v>-555.5555555555555</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2002,6 +2005,176 @@
       </c>
       <c r="E11">
         <v>-555.5555555555555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <v>-1111.111111111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>740.0000000000005</v>
+      </c>
+      <c r="E14">
+        <v>-822.2222222222229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>359.9999999999995</v>
+      </c>
+      <c r="E15">
+        <v>-399.9999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>190.0000000000007</v>
+      </c>
+      <c r="E16">
+        <v>-211.1111111111119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>859.9999999999994</v>
+      </c>
+      <c r="E17">
+        <v>-955.555555555555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>950.0000000000002</v>
+      </c>
+      <c r="E19">
+        <v>-1055.555555555556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>